<commit_message>
Added Use case diagram
</commit_message>
<xml_diff>
--- a/Documentation/Gantt_Chart.xlsx
+++ b/Documentation/Gantt_Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\COEP_TY\A_SEM_6\SE-2\Project\SEMP-II\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C15ABEF-C417-4E16-A193-545D65741185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960C3CA9-113D-443C-9817-9FB6C693DDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F492882C-806F-48FA-9455-1D7CA2D982A5}"/>
   </bookViews>
@@ -1719,7 +1719,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1966,7 +1966,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="17">
-        <f t="shared" si="1"/>
+        <f>C11+1</f>
         <v>44631</v>
       </c>
       <c r="C12" s="15">

</xml_diff>